<commit_message>
Added new test cases forChange password from profile
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\UpNorway_New\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RoshikaG\UPN New\UPN_Insider_App\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C825C983-0C10-4170-BD1E-398BABD5494D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1D3747-D873-4014-8858-FDA4F4E15481}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10960" tabRatio="911" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="changeName_happyPath" sheetId="9" r:id="rId1"/>
     <sheet name="profileChangeValidations" sheetId="77" r:id="rId2"/>
+    <sheet name="checkChangePasswordValidation" sheetId="78" r:id="rId3"/>
+    <sheet name="changePasswordHappyPath" sheetId="79" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>Y</t>
   </si>
@@ -71,16 +73,72 @@
   </si>
   <si>
     <t>(((</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>currentpwd</t>
+  </si>
+  <si>
+    <t>newpwd</t>
+  </si>
+  <si>
+    <t>confirmpwd</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Current password is incorrect</t>
+  </si>
+  <si>
+    <t>Abcd@1234</t>
+  </si>
+  <si>
+    <t>Your password must contain minimum 8 characters</t>
+  </si>
+  <si>
+    <t>Intel@123</t>
+  </si>
+  <si>
+    <t>abcdefgh</t>
+  </si>
+  <si>
+    <t>Your password must contain uppercase and numeric characters</t>
+  </si>
+  <si>
+    <t>Passwords you provided doesn't match</t>
+  </si>
+  <si>
+    <t>Abcd@123</t>
+  </si>
+  <si>
+    <t>Password changed!You successfully changed your password.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,13 +161,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,12 +453,12 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -408,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -419,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -430,7 +491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -438,10 +499,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -461,13 +522,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E313AB86-FBAC-47C9-BF52-892C7B013052}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -478,12 +539,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -494,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>666</v>
       </c>
@@ -508,4 +569,177 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBC9F92-E2C1-47D5-B3D5-1037EAC94786}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{487E307C-0951-400C-B897-43C08BED7033}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{212EC3A8-BC70-4CF8-A57B-F716FE184C23}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{BEF12C46-DE68-4062-8CF5-13B3E2201699}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{D366DB3E-131E-4FE1-BD53-9029A1B556A7}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{B166586F-FCD0-48F1-B3E9-2E9107AE667D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFFE3B1-4CE7-44A8-BD13-147685A76822}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="53.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{24A3539C-5A99-4270-B584-1B3C158F87BD}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{51CCF482-57EC-4715-A578-D368B55C9EBA}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{163B927D-0521-4E01-8863-20DDDB5ABF6A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new test cases for login
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,15 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RoshikaG\UPN New\UPN_Insider_App\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1D3747-D873-4014-8858-FDA4F4E15481}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642BE519-69F6-4C32-B5D0-BF70D776C9B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10960" tabRatio="911" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10960" tabRatio="911" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="changeName_happyPath" sheetId="9" r:id="rId1"/>
     <sheet name="profileChangeValidations" sheetId="77" r:id="rId2"/>
     <sheet name="checkChangePasswordValidation" sheetId="78" r:id="rId3"/>
     <sheet name="changePasswordHappyPath" sheetId="79" r:id="rId4"/>
+    <sheet name="emailValidation_ForgotPassword" sheetId="81" r:id="rId5"/>
+    <sheet name="attemptError_ForgotPassword" sheetId="82" r:id="rId6"/>
+    <sheet name="emptyCode_ForgotPassword" sheetId="83" r:id="rId7"/>
+    <sheet name="nullEmail_Login" sheetId="84" r:id="rId8"/>
+    <sheet name="nullPassword_Login" sheetId="85" r:id="rId9"/>
+    <sheet name="validation_Login" sheetId="86" r:id="rId10"/>
+    <sheet name="successfully_Login" sheetId="87" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="52">
   <si>
     <t>Y</t>
   </si>
@@ -75,7 +82,7 @@
     <t>(((</t>
   </si>
   <si>
-    <t>N</t>
+    <t>email</t>
   </si>
   <si>
     <t>currentpwd</t>
@@ -121,6 +128,69 @@
   </si>
   <si>
     <t>Password changed!You successfully changed your password.</t>
+  </si>
+  <si>
+    <t>This user doesn't exist, please try again with a different email</t>
+  </si>
+  <si>
+    <t>test@abc.com</t>
+  </si>
+  <si>
+    <t>Please enter your email to continue</t>
+  </si>
+  <si>
+    <t>test@abcd.com</t>
+  </si>
+  <si>
+    <t>Attempt limit exceeded, please try after some time.</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>roshikag@99x.lk</t>
+  </si>
+  <si>
+    <t>Please enter your confirmation code to continue</t>
+  </si>
+  <si>
+    <t>Invalid verification code provided, please try again.</t>
+  </si>
+  <si>
+    <t>npwd</t>
+  </si>
+  <si>
+    <t>cpwd</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Please provide your email to continue</t>
+  </si>
+  <si>
+    <t>Please provide your password to continue</t>
+  </si>
+  <si>
+    <t>abc@qwe.com</t>
+  </si>
+  <si>
+    <t>abcd@1234</t>
+  </si>
+  <si>
+    <t>Incorrect email or password.</t>
+  </si>
+  <si>
+    <t>Up Admin</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>roshikaG@99x.lk</t>
+  </si>
+  <si>
+    <t>ROSHIKAG@99X.LK</t>
   </si>
 </sst>
 </file>
@@ -450,235 +520,512 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{457EA7F8-9762-4FD5-9371-D95D8438895D}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{B6548A80-E9B6-4797-B8D2-3AF4D4F6023F}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{A4402EAF-E497-4983-ABB1-60DCB28C468F}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{FFACA390-9A5E-45C9-B25E-3FF657330231}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{E54ED3A1-5E61-4F83-813B-82C98FCC23AE}"/>
+    <hyperlink ref="A3" r:id="rId6" xr:uid="{90C64B96-840C-4438-A491-9ED1BBA9B007}"/>
+    <hyperlink ref="A4" r:id="rId7" xr:uid="{F9EAF352-AAB4-495B-9F94-47A59FD5D3F9}"/>
+    <hyperlink ref="A5" r:id="rId8" xr:uid="{32626DE6-7D38-4A56-ABD0-F6AE064CF45A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2FFA03-7848-4E50-828F-63AABFAB49E8}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" customWidth="1"/>
+    <col min="3" max="3" width="52.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AA0F7114-CD85-44BE-8811-EFF7DA44445B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{F0DA9469-DC3D-47EC-8848-E38966ED15A2}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{91970649-E240-47A7-93D4-01861098677F}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{94FF526A-4C16-47A3-B0BC-D7DE2E6EA68E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7C7999-CA79-40A7-A150-9D602AF01E8C}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{94969142-7624-4BA8-AD2D-E14932AF3BED}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{248A4A22-1FF4-4EAB-8D03-649F6B00C90B}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{5D99AB65-E639-49BA-A75F-03AFB9B7F2D4}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{C0A621B4-CC96-43FE-A190-75249B7CF9A8}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{95C33A48-5BAE-4776-9765-A274BA7863C0}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{B859AF72-2938-43E9-801A-F3716AA0406E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E313AB86-FBAC-47C9-BF52-892C7B013052}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>666</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F95D080B-0354-4AD6-9F05-A1B593E173EE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{02685C7E-2B89-4CD5-AE45-0A63E7B9CE0D}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{0A53FA1A-5236-45F9-B0BC-EAC15CD5B650}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{2B9CB4FD-08BC-4663-A6F4-DCE2FC19F9FC}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{A4625FE3-0161-4C7E-AE8D-4E77AB0CCC71}"/>
+    <hyperlink ref="A3" r:id="rId6" xr:uid="{D966FA59-955F-4A1F-9018-05C03FB09C37}"/>
+    <hyperlink ref="A4" r:id="rId7" xr:uid="{45497525-A623-46F4-9CC9-58D0393E6876}"/>
+    <hyperlink ref="A5" r:id="rId8" xr:uid="{22C865F5-51AC-494F-9176-E05B9896B061}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E313AB86-FBAC-47C9-BF52-892C7B013052}">
-  <dimension ref="A1:C4"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBC9F92-E2C1-47D5-B3D5-1037EAC94786}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>666</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBC9F92-E2C1-47D5-B3D5-1037EAC94786}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="45.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{487E307C-0951-400C-B897-43C08BED7033}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{212EC3A8-BC70-4CF8-A57B-F716FE184C23}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{BEF12C46-DE68-4062-8CF5-13B3E2201699}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{D366DB3E-131E-4FE1-BD53-9029A1B556A7}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{B166586F-FCD0-48F1-B3E9-2E9107AE667D}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{487E307C-0951-400C-B897-43C08BED7033}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{212EC3A8-BC70-4CF8-A57B-F716FE184C23}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{BEF12C46-DE68-4062-8CF5-13B3E2201699}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{D366DB3E-131E-4FE1-BD53-9029A1B556A7}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{B166586F-FCD0-48F1-B3E9-2E9107AE667D}"/>
+    <hyperlink ref="A2" r:id="rId6" xr:uid="{E5D09B2C-2E0A-4039-A44C-8CC2AB673450}"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{0B7CC4B6-1C31-439D-AC3E-12885C8C51C2}"/>
+    <hyperlink ref="B3" r:id="rId8" xr:uid="{16B19A17-F156-41A0-B4FF-EAD0A9AD3408}"/>
+    <hyperlink ref="B4" r:id="rId9" xr:uid="{5618A43E-16AA-4288-A277-46450D58C587}"/>
+    <hyperlink ref="B5" r:id="rId10" xr:uid="{C867775A-05DC-4337-A798-63A0707AE4DE}"/>
+    <hyperlink ref="A3" r:id="rId11" xr:uid="{08E23D02-ADCD-4C63-B162-792B7F775785}"/>
+    <hyperlink ref="A4" r:id="rId12" xr:uid="{3AC1CA1E-B2CC-48EE-8B3D-9B88DBB188AF}"/>
+    <hyperlink ref="A5" r:id="rId13" xr:uid="{2B2B69F2-7811-4D30-8B0F-42DDE5ED3140}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -686,40 +1033,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFFE3B1-4CE7-44A8-BD13-147685A76822}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="53.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="53.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
@@ -727,19 +1082,307 @@
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{24A3539C-5A99-4270-B584-1B3C158F87BD}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{51CCF482-57EC-4715-A578-D368B55C9EBA}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{163B927D-0521-4E01-8863-20DDDB5ABF6A}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{24A3539C-5A99-4270-B584-1B3C158F87BD}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{51CCF482-57EC-4715-A578-D368B55C9EBA}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{163B927D-0521-4E01-8863-20DDDB5ABF6A}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{829853FC-CE02-4AE7-B30A-F9B641E46667}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{2FBB1043-D244-4401-884B-603F1E4C2D8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE71EE4-15C1-463F-8275-DC8357C2DB89}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="52.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2C587C48-9066-4BC9-94AA-9D83CEDCE673}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC742D8-4FB5-4FE0-8ECB-39C0FF36FA9B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" customWidth="1"/>
+    <col min="2" max="2" width="45.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{55AB346C-32EE-4980-AA4E-4925F74229E3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA035BF0-2224-4214-BDCE-42004819E6ED}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+    <col min="5" max="5" width="44.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>123456</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6110FFB4-28DD-428F-8CDF-16AB47025B8E}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{4526E02E-8193-4518-B951-26B2F2D733C0}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{9DAB12AD-1DAC-4410-9F26-EE061FB5DB17}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{C57E5BB1-8830-4916-9570-19DCB33813BA}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{9AEF12AD-3E7D-4B52-8625-03C3CE95911D}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{753AF0ED-E8F7-41DB-9F3F-014467F62228}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFF4DAA-0A1E-4DA8-83ED-6511C9DA305A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="3" max="3" width="59.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D57FB471-5EEA-443C-8E60-FCDD5366E609}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E37AB3-5BAA-40B4-AC57-1D705293F014}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D4A80B7A-E42E-43D3-A5EB-ABC3F6E5DCD5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated the environment as staging
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RoshikaG\UPN New\UPN_Insider_App\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642BE519-69F6-4C32-B5D0-BF70D776C9B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A469F24A-9609-44C5-BCD8-9DAF4D809EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10960" tabRatio="911" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10960" tabRatio="911" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="changeName_happyPath" sheetId="9" r:id="rId1"/>
@@ -522,8 +522,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,7 +637,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBC9F92-E2C1-47D5-B3D5-1037EAC94786}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1036,7 +1036,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added new test cases for Insider Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RoshikaG\UPN New\UPN_Insider_App\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A469F24A-9609-44C5-BCD8-9DAF4D809EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCB95BB-6166-4F2B-9C88-EC8453E405A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10960" tabRatio="911" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10960" tabRatio="911" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="changeName_happyPath" sheetId="9" r:id="rId1"/>
@@ -24,6 +24,9 @@
     <sheet name="nullPassword_Login" sheetId="85" r:id="rId9"/>
     <sheet name="validation_Login" sheetId="86" r:id="rId10"/>
     <sheet name="successfully_Login" sheetId="87" r:id="rId11"/>
+    <sheet name="viewAll_ChatNotifications" sheetId="88" r:id="rId12"/>
+    <sheet name="checkNotificationMenu" sheetId="89" r:id="rId13"/>
+    <sheet name="checkRemindersMenu" sheetId="90" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="56">
   <si>
     <t>Y</t>
   </si>
@@ -191,6 +194,18 @@
   </si>
   <si>
     <t>ROSHIKAG@99X.LK</t>
+  </si>
+  <si>
+    <t>Here Are your Messages</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>Reminders</t>
   </si>
 </sst>
 </file>
@@ -705,7 +720,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -778,6 +793,167 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{C0A621B4-CC96-43FE-A190-75249B7CF9A8}"/>
     <hyperlink ref="A4" r:id="rId5" xr:uid="{95C33A48-5BAE-4776-9765-A274BA7863C0}"/>
     <hyperlink ref="B4" r:id="rId6" xr:uid="{B859AF72-2938-43E9-801A-F3716AA0406E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D5F047-2551-4B30-83EB-E57D257AA40B}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="29.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0705AB53-3302-4615-B2C3-FF594D3BB119}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{3F9F88D1-9256-43A0-BC8B-161C08B4CDCF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA41B5B-1AAC-4635-8A80-7419B6B767A6}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D6CD7D72-4B76-4496-BB71-1B9F30DAF309}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{8D78AA0C-C363-48E4-AA49-50B2AE570036}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072492E4-1D77-4B13-989F-340352462F1A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{820BDBF3-AB58-4117-8E70-D81F988BCC4A}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C461CECD-BF81-43D9-ADAB-1608CC8AC78A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -882,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBC9F92-E2C1-47D5-B3D5-1037EAC94786}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added partner test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RoshikaG\UPN New\UPN_Insider_App\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\UpNorway_New\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCB95BB-6166-4F2B-9C88-EC8453E405A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FCB805-09EC-4FC9-93C1-F561D665ECCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10960" tabRatio="911" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="changeName_happyPath" sheetId="9" r:id="rId1"/>
@@ -27,6 +27,9 @@
     <sheet name="viewAll_ChatNotifications" sheetId="88" r:id="rId12"/>
     <sheet name="checkNotificationMenu" sheetId="89" r:id="rId13"/>
     <sheet name="checkRemindersMenu" sheetId="90" r:id="rId14"/>
+    <sheet name="addNewPartner" sheetId="91" r:id="rId15"/>
+    <sheet name="AddPartnerFieldValidation" sheetId="93" r:id="rId16"/>
+    <sheet name="Sheet2" sheetId="92" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="88">
   <si>
     <t>Y</t>
   </si>
@@ -206,6 +209,102 @@
   </si>
   <si>
     <t>Reminders</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>contactpersonadmin</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>postalcode</t>
+  </si>
+  <si>
+    <t>postcity</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Travel SL</t>
+  </si>
+  <si>
+    <t>Dialog</t>
+  </si>
+  <si>
+    <t>Sanath</t>
+  </si>
+  <si>
+    <t>sanath@gmail.com</t>
+  </si>
+  <si>
+    <t>Coloimbo</t>
+  </si>
+  <si>
+    <t>Colombo</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>3333</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>travelsl.com</t>
+  </si>
+  <si>
+    <t>src/test/resources/images/img1.jpg</t>
+  </si>
+  <si>
+    <t>+4712345678</t>
+  </si>
+  <si>
+    <t>contactpersonbooking</t>
+  </si>
+  <si>
+    <t>emailbooking</t>
+  </si>
+  <si>
+    <t>phonebooking</t>
+  </si>
+  <si>
+    <t>Malinga</t>
+  </si>
+  <si>
+    <t>ma@sl.com</t>
+  </si>
+  <si>
+    <t>contacttype</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>Item added successfully!</t>
+  </si>
+  <si>
+    <t>toastmessage</t>
   </si>
 </sst>
 </file>
@@ -250,9 +349,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -541,13 +642,13 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -564,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -581,7 +682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -598,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -615,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -655,14 +756,14 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" customWidth="1"/>
-    <col min="3" max="3" width="52.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="52.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -676,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -690,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -723,13 +824,13 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -743,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -757,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
@@ -771,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -806,12 +907,12 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="29.36328125" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -828,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -863,14 +964,14 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.90625" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -884,7 +985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -911,18 +1012,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072492E4-1D77-4B13-989F-340352462F1A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -936,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -959,6 +1060,294 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E78B0E-4A2F-4D35-9C82-6433A6DC0EBA}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{DEBCF645-9D83-4187-AF9E-8379F12A78C9}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{7389FA25-1675-4283-BEE4-D278A65A395B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0411333-0C39-4C29-8D7C-AAB5FDC99DF1}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{E82A1D55-3223-42CB-BAD7-BCF76D56FE4D}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{E4EE1275-9F71-4049-839D-54160390CC44}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE385B87-165B-45A8-93A5-183944A56A90}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E313AB86-FBAC-47C9-BF52-892C7B013052}">
   <dimension ref="A1:E5"/>
@@ -967,9 +1356,9 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -986,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -997,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -1014,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -1031,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1062,17 +1451,17 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" customWidth="1"/>
-    <col min="6" max="6" width="45.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="45.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1095,7 +1484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1118,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -1141,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -1164,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1215,17 +1604,17 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="53.36328125" customWidth="1"/>
+    <col min="6" max="6" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1248,7 +1637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1291,13 +1680,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="52.6328125" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1308,7 +1697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -1319,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -1343,13 +1732,13 @@
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="2" width="45.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="45.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1360,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1387,15 +1776,15 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" customWidth="1"/>
-    <col min="5" max="5" width="44.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="44.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1415,7 +1804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1433,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -1474,14 +1863,14 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="59.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1495,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1522,13 +1911,13 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1542,7 +1931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
more test cases on activities and items
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\UpNorway_New\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3CA066-B998-4F8C-A2A4-C607E6F22AEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D4FA74-82FB-4A92-8CEF-3518F7780A9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" firstSheet="18" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="changeName_happyPath" sheetId="9" r:id="rId1"/>
@@ -30,6 +30,13 @@
     <sheet name="add_New_Partner" sheetId="91" r:id="rId15"/>
     <sheet name="Add_Partner_Field_Validation" sheetId="93" r:id="rId16"/>
     <sheet name="update_Partner_Company_Info" sheetId="92" r:id="rId17"/>
+    <sheet name="update_partner_agreeement_info" sheetId="94" r:id="rId18"/>
+    <sheet name="upload_partner_agreement" sheetId="95" r:id="rId19"/>
+    <sheet name="Add_new_activity" sheetId="96" r:id="rId20"/>
+    <sheet name="update_activity_template" sheetId="97" r:id="rId21"/>
+    <sheet name="add_new_item" sheetId="98" r:id="rId22"/>
+    <sheet name="edit_item_template" sheetId="99" r:id="rId23"/>
+    <sheet name="add_another_item" sheetId="101" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="165">
   <si>
     <t>Y</t>
   </si>
@@ -382,6 +389,168 @@
   </si>
   <si>
     <t>EMAIL</t>
+  </si>
+  <si>
+    <t>bookingtype</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>generalnotes</t>
+  </si>
+  <si>
+    <t>google.com</t>
+  </si>
+  <si>
+    <t>larry</t>
+  </si>
+  <si>
+    <t>rajapaksa</t>
+  </si>
+  <si>
+    <t>very good partner to deal with</t>
+  </si>
+  <si>
+    <t>DIRECT</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>src/test/resources/images/test.pdf</t>
+  </si>
+  <si>
+    <t>documentname</t>
+  </si>
+  <si>
+    <t>The uploaded file will appear in agreements soon</t>
+  </si>
+  <si>
+    <t>Ag13</t>
+  </si>
+  <si>
+    <t>activityType</t>
+  </si>
+  <si>
+    <t>activityimage</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>Flight</t>
+  </si>
+  <si>
+    <t>Colombo to Norway</t>
+  </si>
+  <si>
+    <t>Activity added successfully!</t>
+  </si>
+  <si>
+    <t>src/test/resources/images/logo-color.png</t>
+  </si>
+  <si>
+    <t>Activity updated successfully!</t>
+  </si>
+  <si>
+    <t>Updated the description 1</t>
+  </si>
+  <si>
+    <t>itemname</t>
+  </si>
+  <si>
+    <t>priceoption</t>
+  </si>
+  <si>
+    <t>op1_upn_price</t>
+  </si>
+  <si>
+    <t>op1_vat_rate</t>
+  </si>
+  <si>
+    <t>op1_marketprice</t>
+  </si>
+  <si>
+    <t>op1_commission</t>
+  </si>
+  <si>
+    <t>arshad_iitem_1_fixed_price</t>
+  </si>
+  <si>
+    <t>op2_marketpricechild</t>
+  </si>
+  <si>
+    <t>op3_priceroom</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>PERSON</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>ROOM</t>
+  </si>
+  <si>
+    <t>arshad_iitem_3_Room</t>
+  </si>
+  <si>
+    <t>arshad_iitem_2_Person</t>
+  </si>
+  <si>
+    <t>long desc long desc long desc long desc long desc long desc long desc long desc long desc long desc</t>
+  </si>
+  <si>
+    <t>Recently UpdatedRecently UpdatedRecently UpdatedRecently Updated Recently Updated Recently UpdatedRecently UpdatedRecently UpdatedRecently UpdatedRecently Updated</t>
+  </si>
+  <si>
+    <t>Only My Issues Only My Issues Only My Issues Only My Issues Only My Issues Only My Issues Only My Issues Only My Issues Only My Issues</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>567</t>
+  </si>
+  <si>
+    <t>op2_marketpriceadult</t>
+  </si>
+  <si>
+    <t>nothing much to say2</t>
+  </si>
+  <si>
+    <t>India to US</t>
+  </si>
+  <si>
+    <t>Second iteration</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1458,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1450,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE385B87-165B-45A8-93A5-183944A56A90}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1603,6 +1772,104 @@
     <hyperlink ref="G2" r:id="rId1" xr:uid="{162335B4-2322-4D4A-81F6-DE199EB280F6}"/>
     <hyperlink ref="J2" r:id="rId2" xr:uid="{64D17E7C-F599-46D9-9650-63562FD400B8}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E7CCFE-5DCA-46C4-A5B9-3111AE2797FF}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7410968-923A-44CA-9021-36A424E38FAB}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1698,6 +1965,324 @@
     <hyperlink ref="A4" r:id="rId7" xr:uid="{45497525-A623-46F4-9CC9-58D0393E6876}"/>
     <hyperlink ref="A5" r:id="rId8" xr:uid="{22C865F5-51AC-494F-9176-E05B9896B061}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD7C2CD-6937-42E8-B7B9-7454600C1D42}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB174383-F750-445C-A525-F4FB8D78441A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5232F7E8-3361-4283-83CF-3D53020EF6C2}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.77734375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6ACAA9-BD1E-45FA-84A2-FBEBDEEFB58F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C06169-9837-458E-BE0E-EFEE8DD3433D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>